<commit_message>
chore: add date format in attendance template
</commit_message>
<xml_diff>
--- a/public/attendance_time_data.xlsx
+++ b/public/attendance_time_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,18 +413,21 @@
         <v>employee_code</v>
       </c>
       <c r="D1" t="str">
+        <v>date</v>
+      </c>
+      <c r="E1" t="str">
         <v>in</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>out</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>status</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(attendance-import): fix import attendance
</commit_message>
<xml_diff>
--- a/public/attendance_time_data.xlsx
+++ b/public/attendance_time_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,7 +410,7 @@
         <v>branch_code</v>
       </c>
       <c r="C1" t="str">
-        <v>employee_code</v>
+        <v>nik</v>
       </c>
       <c r="D1" t="str">
         <v>date</v>
@@ -423,11 +423,34 @@
       </c>
       <c r="G1" t="str">
         <v>status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>WCK760</v>
+      </c>
+      <c r="B2" t="str">
+        <v>SIF141</v>
+      </c>
+      <c r="C2" t="str">
+        <v>123123</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2023-10-01</v>
+      </c>
+      <c r="E2" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="F2" t="str">
+        <v>18:00</v>
+      </c>
+      <c r="G2" t="str">
+        <v>on time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>